<commit_message>
cost optimizer in development
</commit_message>
<xml_diff>
--- a/Datos_Entregable2_Hackathon_predicted.xlsx
+++ b/Datos_Entregable2_Hackathon_predicted.xlsx
@@ -1,62 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mico\Desktop\deep learning\desafios\hackathon-enaex-2019\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A8D578-C2B6-41C9-B953-4A4899A4A456}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P20</t>
-  </si>
-  <si>
-    <t>P30</t>
-  </si>
-  <si>
-    <t>P40</t>
-  </si>
-  <si>
-    <t>P50</t>
-  </si>
-  <si>
-    <t>P60</t>
-  </si>
-  <si>
-    <t>P70</t>
-  </si>
-  <si>
-    <t>P80</t>
-  </si>
-  <si>
-    <t>P90</t>
-  </si>
-  <si>
-    <t>P100</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,19 +78,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -173,7 +124,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,27 +156,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,24 +190,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,781 +365,779 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
-        <v>0.48588329553604132</v>
+        <v>0.601481020450592</v>
       </c>
       <c r="B2">
-        <v>0.88924652338027954</v>
+        <v>1.030508756637573</v>
       </c>
       <c r="C2">
-        <v>1.302193164825439</v>
+        <v>1.411880016326904</v>
       </c>
       <c r="D2">
-        <v>1.5770876407623291</v>
+        <v>1.96860134601593</v>
       </c>
       <c r="E2">
-        <v>1.938382148742676</v>
+        <v>2.543120622634888</v>
       </c>
       <c r="F2">
-        <v>2.5838572978973389</v>
+        <v>3.30126166343689</v>
       </c>
       <c r="G2">
-        <v>3.3465569019317631</v>
+        <v>4.346879482269287</v>
       </c>
       <c r="H2">
-        <v>4.3764257431030273</v>
+        <v>5.369348526000977</v>
       </c>
       <c r="I2">
-        <v>6.0170059204101563</v>
+        <v>7.233903884887695</v>
       </c>
       <c r="J2">
-        <v>10.901017189025881</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.68030452728271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
-        <v>0.43678450584411621</v>
+        <v>0.3538975119590759</v>
       </c>
       <c r="B3">
-        <v>0.75349074602127075</v>
+        <v>0.6662895083427429</v>
       </c>
       <c r="C3">
-        <v>1.100860118865967</v>
+        <v>0.8295960426330566</v>
       </c>
       <c r="D3">
-        <v>1.418016195297241</v>
+        <v>1.094967603683472</v>
       </c>
       <c r="E3">
-        <v>1.8409889936447139</v>
+        <v>1.586832761764526</v>
       </c>
       <c r="F3">
-        <v>2.409356832504272</v>
+        <v>2.031749963760376</v>
       </c>
       <c r="G3">
-        <v>3.1434609889984131</v>
+        <v>2.708300828933716</v>
       </c>
       <c r="H3">
-        <v>4.0512404441833496</v>
+        <v>3.744156360626221</v>
       </c>
       <c r="I3">
-        <v>5.508018970489502</v>
+        <v>4.983140468597412</v>
       </c>
       <c r="J3">
-        <v>9.9218721389770508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.02602481842041</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
-        <v>0.47590148448944092</v>
+        <v>0.4899917840957642</v>
       </c>
       <c r="B4">
-        <v>0.85931861400604248</v>
+        <v>0.8582075834274292</v>
       </c>
       <c r="C4">
-        <v>1.22913670539856</v>
+        <v>1.295301556587219</v>
       </c>
       <c r="D4">
-        <v>1.6455532312393191</v>
+        <v>1.716436147689819</v>
       </c>
       <c r="E4">
-        <v>2.0804374217987061</v>
+        <v>2.191340208053589</v>
       </c>
       <c r="F4">
-        <v>2.589471578598022</v>
+        <v>2.692466259002686</v>
       </c>
       <c r="G4">
-        <v>3.1905171871185298</v>
+        <v>3.345820903778076</v>
       </c>
       <c r="H4">
-        <v>3.9386367797851558</v>
+        <v>4.029809474945068</v>
       </c>
       <c r="I4">
-        <v>5.123469352722168</v>
+        <v>5.131371974945068</v>
       </c>
       <c r="J4">
-        <v>8.705378532409668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.312727928161621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
-        <v>0.47575408220291138</v>
+        <v>0.4898808598518372</v>
       </c>
       <c r="B5">
-        <v>0.8591151237487793</v>
+        <v>0.8581814169883728</v>
       </c>
       <c r="C5">
-        <v>1.229131698608398</v>
+        <v>1.29522693157196</v>
       </c>
       <c r="D5">
-        <v>1.644977331161499</v>
+        <v>1.716400146484375</v>
       </c>
       <c r="E5">
-        <v>2.0798087120056148</v>
+        <v>2.191296577453613</v>
       </c>
       <c r="F5">
-        <v>2.588772058486938</v>
+        <v>2.692446231842041</v>
       </c>
       <c r="G5">
-        <v>3.1898503303527832</v>
+        <v>3.34578275680542</v>
       </c>
       <c r="H5">
-        <v>3.937548160552979</v>
+        <v>4.029992580413818</v>
       </c>
       <c r="I5">
-        <v>5.1217198371887207</v>
+        <v>5.131570339202881</v>
       </c>
       <c r="J5">
-        <v>8.7011852264404297</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.313373565673828</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
-        <v>0.46738868951797491</v>
+        <v>0.5008202195167542</v>
       </c>
       <c r="B6">
-        <v>0.83390450477600098</v>
+        <v>0.8929207324981689</v>
       </c>
       <c r="C6">
-        <v>1.171389579772949</v>
+        <v>1.272610783576965</v>
       </c>
       <c r="D6">
-        <v>1.5256937742233281</v>
+        <v>1.666047811508179</v>
       </c>
       <c r="E6">
-        <v>1.9407311677932739</v>
+        <v>2.193484306335449</v>
       </c>
       <c r="F6">
-        <v>2.467532873153687</v>
+        <v>2.757428169250488</v>
       </c>
       <c r="G6">
-        <v>3.1376128196716309</v>
+        <v>3.464641094207764</v>
       </c>
       <c r="H6">
-        <v>3.9639265537261958</v>
+        <v>4.241957664489746</v>
       </c>
       <c r="I6">
-        <v>5.2669029235839844</v>
+        <v>5.353704929351807</v>
       </c>
       <c r="J6">
-        <v>9.3076486587524414</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.743186950683594</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
-        <v>0.47607111930847168</v>
+        <v>0.4901056289672852</v>
       </c>
       <c r="B7">
-        <v>0.85955500602722168</v>
+        <v>0.8582290410995483</v>
       </c>
       <c r="C7">
-        <v>1.2291626930236821</v>
+        <v>1.295375227928162</v>
       </c>
       <c r="D7">
-        <v>1.646211981773376</v>
+        <v>1.716463088989258</v>
       </c>
       <c r="E7">
-        <v>2.0811560153961182</v>
+        <v>2.191376209259033</v>
       </c>
       <c r="F7">
-        <v>2.5902690887451172</v>
+        <v>2.6924729347229</v>
       </c>
       <c r="G7">
-        <v>3.191281795501709</v>
+        <v>3.345842838287354</v>
       </c>
       <c r="H7">
-        <v>3.939872264862061</v>
+        <v>4.029593944549561</v>
       </c>
       <c r="I7">
-        <v>5.1254391670227051</v>
+        <v>5.131137371063232</v>
       </c>
       <c r="J7">
-        <v>8.7100744247436523</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.311985015869141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
-        <v>0.47597628831863398</v>
+        <v>0.4900673031806946</v>
       </c>
       <c r="B8">
-        <v>0.85941922664642334</v>
+        <v>0.8582383990287781</v>
       </c>
       <c r="C8">
-        <v>1.229145288467407</v>
+        <v>1.295360088348389</v>
       </c>
       <c r="D8">
-        <v>1.6458500623703001</v>
+        <v>1.716482639312744</v>
       </c>
       <c r="E8">
-        <v>2.0807628631591801</v>
+        <v>2.191388845443726</v>
       </c>
       <c r="F8">
-        <v>2.5898313522338872</v>
+        <v>2.692512273788452</v>
       </c>
       <c r="G8">
-        <v>3.1908624172210689</v>
+        <v>3.345886468887329</v>
       </c>
       <c r="H8">
-        <v>3.939194917678833</v>
+        <v>4.029745578765869</v>
       </c>
       <c r="I8">
-        <v>5.1243624687194824</v>
+        <v>5.13130521774292</v>
       </c>
       <c r="J8">
-        <v>8.7074871063232422</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.312465667724609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
-        <v>0.47583401203155518</v>
+        <v>0.4899821281433105</v>
       </c>
       <c r="B9">
-        <v>0.85922127962112427</v>
+        <v>0.8582297563552856</v>
       </c>
       <c r="C9">
-        <v>1.2291285991668699</v>
+        <v>1.295308709144592</v>
       </c>
       <c r="D9">
-        <v>1.6453007459640501</v>
+        <v>1.716475248336792</v>
       </c>
       <c r="E9">
-        <v>2.0801653861999512</v>
+        <v>2.191372632980347</v>
       </c>
       <c r="F9">
-        <v>2.5891683101654048</v>
+        <v>2.692526817321777</v>
       </c>
       <c r="G9">
-        <v>3.190228939056396</v>
+        <v>3.345893383026123</v>
       </c>
       <c r="H9">
-        <v>3.9381670951843262</v>
+        <v>4.029942035675049</v>
       </c>
       <c r="I9">
-        <v>5.1227188110351563</v>
+        <v>5.131520748138428</v>
       </c>
       <c r="J9">
-        <v>8.7035493850708008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.31312084197998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
-        <v>0.47577863931655878</v>
+        <v>0.4899479746818542</v>
       </c>
       <c r="B10">
-        <v>0.85914289951324463</v>
+        <v>0.8582261800765991</v>
       </c>
       <c r="C10">
-        <v>1.2291276454925539</v>
+        <v>1.295289397239685</v>
       </c>
       <c r="D10">
-        <v>1.6450874805450439</v>
+        <v>1.716472744941711</v>
       </c>
       <c r="E10">
-        <v>2.0799319744110112</v>
+        <v>2.191366672515869</v>
       </c>
       <c r="F10">
-        <v>2.5889074802398682</v>
+        <v>2.692532777786255</v>
       </c>
       <c r="G10">
-        <v>3.1899814605712891</v>
+        <v>3.34589695930481</v>
       </c>
       <c r="H10">
-        <v>3.9377613067626949</v>
+        <v>4.030022144317627</v>
       </c>
       <c r="I10">
-        <v>5.1220664978027344</v>
+        <v>5.131608486175537</v>
       </c>
       <c r="J10">
-        <v>8.7019767761230469</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.313386917114258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
-        <v>0.46711397171020508</v>
+        <v>0.5008254647254944</v>
       </c>
       <c r="B11">
-        <v>0.83343034982681274</v>
+        <v>0.8919277191162109</v>
       </c>
       <c r="C11">
-        <v>1.171110153198242</v>
+        <v>1.271595239639282</v>
       </c>
       <c r="D11">
-        <v>1.5251526832580571</v>
+        <v>1.665282368659973</v>
       </c>
       <c r="E11">
-        <v>1.940747022628784</v>
+        <v>2.191754817962646</v>
       </c>
       <c r="F11">
-        <v>2.4674274921417241</v>
+        <v>2.755521297454834</v>
       </c>
       <c r="G11">
-        <v>3.1374192237853999</v>
+        <v>3.462100982666016</v>
       </c>
       <c r="H11">
-        <v>3.9626247882843022</v>
+        <v>4.238498687744141</v>
       </c>
       <c r="I11">
-        <v>5.2638731002807617</v>
+        <v>5.350760459899902</v>
       </c>
       <c r="J11">
-        <v>9.2963056564331055</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.740213394165039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
-        <v>0.46695113182067871</v>
+        <v>0.5015303492546082</v>
       </c>
       <c r="B12">
-        <v>0.83314251899719238</v>
+        <v>0.8927595615386963</v>
       </c>
       <c r="C12">
-        <v>1.1710584163665769</v>
+        <v>1.272670865058899</v>
       </c>
       <c r="D12">
-        <v>1.525224089622498</v>
+        <v>1.666847825050354</v>
       </c>
       <c r="E12">
-        <v>1.940875768661499</v>
+        <v>2.193403244018555</v>
       </c>
       <c r="F12">
-        <v>2.467359304428101</v>
+        <v>2.757736682891846</v>
       </c>
       <c r="G12">
-        <v>3.1372337341308589</v>
+        <v>3.464530944824219</v>
       </c>
       <c r="H12">
-        <v>3.9621727466583252</v>
+        <v>4.240735054016113</v>
       </c>
       <c r="I12">
-        <v>5.2631115913391113</v>
+        <v>5.353139400482178</v>
       </c>
       <c r="J12">
-        <v>9.2929000854492188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.743449211120605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
-        <v>0.44503843784332281</v>
+        <v>0.4212114810943604</v>
       </c>
       <c r="B13">
-        <v>0.80703920125961304</v>
+        <v>0.768099844455719</v>
       </c>
       <c r="C13">
-        <v>1.1296577453613279</v>
+        <v>1.164458036422729</v>
       </c>
       <c r="D13">
-        <v>1.4982122182846069</v>
+        <v>1.526866316795349</v>
       </c>
       <c r="E13">
-        <v>1.92958652973175</v>
+        <v>2.020687103271484</v>
       </c>
       <c r="F13">
-        <v>2.464117288589478</v>
+        <v>2.573098659515381</v>
       </c>
       <c r="G13">
-        <v>3.118525505065918</v>
+        <v>3.228649139404297</v>
       </c>
       <c r="H13">
-        <v>3.9258160591125488</v>
+        <v>4.019401550292969</v>
       </c>
       <c r="I13">
-        <v>5.2067432403564453</v>
+        <v>5.131402969360352</v>
       </c>
       <c r="J13">
-        <v>9.0809707641601563</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.325536727905273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
-        <v>0.44559192657470698</v>
+        <v>0.4900974035263062</v>
       </c>
       <c r="B14">
-        <v>0.79883956909179688</v>
+        <v>0.8703179359436035</v>
       </c>
       <c r="C14">
-        <v>1.104750394821167</v>
+        <v>1.173951148986816</v>
       </c>
       <c r="D14">
-        <v>1.405534625053406</v>
+        <v>1.556616067886353</v>
       </c>
       <c r="E14">
-        <v>1.8014892339706421</v>
+        <v>2.12877345085144</v>
       </c>
       <c r="F14">
-        <v>2.344962358474731</v>
+        <v>2.690981864929199</v>
       </c>
       <c r="G14">
-        <v>3.0490889549255371</v>
+        <v>3.389682292938232</v>
       </c>
       <c r="H14">
-        <v>3.9168791770935059</v>
+        <v>4.349557876586914</v>
       </c>
       <c r="I14">
-        <v>5.2879080772399902</v>
+        <v>5.503628730773926</v>
       </c>
       <c r="J14">
-        <v>9.5970602035522461</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.14129638671875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
-        <v>0.44549697637557978</v>
+        <v>0.4900652170181274</v>
       </c>
       <c r="B15">
-        <v>0.79869866371154785</v>
+        <v>0.870166540145874</v>
       </c>
       <c r="C15">
-        <v>1.1045799255371089</v>
+        <v>1.173757195472717</v>
       </c>
       <c r="D15">
-        <v>1.405298113822937</v>
+        <v>1.556429266929626</v>
       </c>
       <c r="E15">
-        <v>1.801300525665283</v>
+        <v>2.128564357757568</v>
       </c>
       <c r="F15">
-        <v>2.3447892665863042</v>
+        <v>2.690808534622192</v>
       </c>
       <c r="G15">
-        <v>3.0489532947540279</v>
+        <v>3.389420032501221</v>
       </c>
       <c r="H15">
-        <v>3.9166991710662842</v>
+        <v>4.349486351013184</v>
       </c>
       <c r="I15">
-        <v>5.2876791954040527</v>
+        <v>5.503664016723633</v>
       </c>
       <c r="J15">
-        <v>9.5962457656860352</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.141541481018066</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
-        <v>0.46739661693572998</v>
+        <v>0.4530773162841797</v>
       </c>
       <c r="B16">
-        <v>0.85259658098220825</v>
+        <v>0.8398188352584839</v>
       </c>
       <c r="C16">
-        <v>1.223731994628906</v>
+        <v>1.287380695343018</v>
       </c>
       <c r="D16">
-        <v>1.6441711187362671</v>
+        <v>1.688829064369202</v>
       </c>
       <c r="E16">
-        <v>2.0862371921539311</v>
+        <v>2.173237085342407</v>
       </c>
       <c r="F16">
-        <v>2.6023774147033691</v>
+        <v>2.616086959838867</v>
       </c>
       <c r="G16">
-        <v>3.197124719619751</v>
+        <v>3.273769617080688</v>
       </c>
       <c r="H16">
-        <v>3.93678879737854</v>
+        <v>3.976587295532227</v>
       </c>
       <c r="I16">
-        <v>5.1110625267028809</v>
+        <v>5.039022922515869</v>
       </c>
       <c r="J16">
-        <v>8.6271638870239258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.16018009185791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
-        <v>0.40843671560287481</v>
+        <v>0.3913776278495789</v>
       </c>
       <c r="B17">
-        <v>0.69349855184555054</v>
+        <v>0.7029466032981873</v>
       </c>
       <c r="C17">
-        <v>1.075968980789185</v>
+        <v>1.011512875556946</v>
       </c>
       <c r="D17">
-        <v>1.3414046764373779</v>
+        <v>1.29172694683075</v>
       </c>
       <c r="E17">
-        <v>1.7887475490570071</v>
+        <v>1.79174017906189</v>
       </c>
       <c r="F17">
-        <v>2.3914253711700439</v>
+        <v>2.228490829467773</v>
       </c>
       <c r="G17">
-        <v>3.1723687648773189</v>
+        <v>2.943617582321167</v>
       </c>
       <c r="H17">
-        <v>4.0940027236938477</v>
+        <v>3.887405157089233</v>
       </c>
       <c r="I17">
-        <v>5.5873980522155762</v>
+        <v>5.108297824859619</v>
       </c>
       <c r="J17">
-        <v>9.9695835113525391</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.061622619628906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
-        <v>0.43105363845825201</v>
+        <v>0.5200793743133545</v>
       </c>
       <c r="B18">
-        <v>0.72029238939285278</v>
+        <v>0.8131012320518494</v>
       </c>
       <c r="C18">
-        <v>1.1090443134307859</v>
+        <v>1.198380351066589</v>
       </c>
       <c r="D18">
-        <v>1.379595994949341</v>
+        <v>1.623135566711426</v>
       </c>
       <c r="E18">
-        <v>1.7849640846252439</v>
+        <v>2.08718729019165</v>
       </c>
       <c r="F18">
-        <v>2.304787397384644</v>
+        <v>2.709656476974487</v>
       </c>
       <c r="G18">
-        <v>3.0029647350311279</v>
+        <v>3.377738952636719</v>
       </c>
       <c r="H18">
-        <v>3.8186311721801758</v>
+        <v>4.13623571395874</v>
       </c>
       <c r="I18">
-        <v>5.143834114074707</v>
+        <v>5.379188537597656</v>
       </c>
       <c r="J18">
-        <v>9.0499067306518555</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.90714168548584</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
-        <v>0.51183480024337769</v>
+        <v>0.5812098383903503</v>
       </c>
       <c r="B19">
-        <v>0.7791638970375061</v>
+        <v>0.9470065832138062</v>
       </c>
       <c r="C19">
-        <v>1.295362234115601</v>
+        <v>1.425147414207458</v>
       </c>
       <c r="D19">
-        <v>1.373998641967773</v>
+        <v>1.716510057449341</v>
       </c>
       <c r="E19">
-        <v>1.8152586221694951</v>
+        <v>2.126291513442993</v>
       </c>
       <c r="F19">
-        <v>2.504258394241333</v>
+        <v>2.754150152206421</v>
       </c>
       <c r="G19">
-        <v>3.41102147102356</v>
+        <v>3.502137660980225</v>
       </c>
       <c r="H19">
-        <v>4.4010896682739258</v>
+        <v>4.190216064453125</v>
       </c>
       <c r="I19">
-        <v>5.9807209968566886</v>
+        <v>5.675093650817871</v>
       </c>
       <c r="J19">
-        <v>11.16562557220459</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.45807647705078</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
-        <v>0.59335428476333618</v>
+        <v>0.5474885702133179</v>
       </c>
       <c r="B20">
-        <v>1.1006772518157959</v>
+        <v>1.128917694091797</v>
       </c>
       <c r="C20">
-        <v>1.72283411026001</v>
+        <v>1.776350378990173</v>
       </c>
       <c r="D20">
-        <v>2.3563017845153809</v>
+        <v>2.390175342559814</v>
       </c>
       <c r="E20">
-        <v>3.0613961219787602</v>
+        <v>3.134697914123535</v>
       </c>
       <c r="F20">
-        <v>3.868163108825684</v>
+        <v>3.890769243240356</v>
       </c>
       <c r="G20">
-        <v>4.7192678451538086</v>
+        <v>4.733163833618164</v>
       </c>
       <c r="H20">
-        <v>5.7716870307922363</v>
+        <v>5.76230001449585</v>
       </c>
       <c r="I20">
-        <v>7.390068531036377</v>
+        <v>7.146996021270752</v>
       </c>
       <c r="J20">
-        <v>11.603560447692869</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.80641937255859</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
-        <v>0.36623859405517578</v>
+        <v>0.34197598695755</v>
       </c>
       <c r="B21">
-        <v>0.59301543235778809</v>
+        <v>0.785072922706604</v>
       </c>
       <c r="C21">
-        <v>0.92022603750228882</v>
+        <v>1.077635526657104</v>
       </c>
       <c r="D21">
-        <v>1.258864641189575</v>
+        <v>1.489043474197388</v>
       </c>
       <c r="E21">
-        <v>1.755241870880127</v>
+        <v>1.966318964958191</v>
       </c>
       <c r="F21">
-        <v>2.283920049667358</v>
+        <v>2.565984725952148</v>
       </c>
       <c r="G21">
-        <v>2.9835019111633301</v>
+        <v>3.028093099594116</v>
       </c>
       <c r="H21">
-        <v>3.769012451171875</v>
+        <v>3.94559645652771</v>
       </c>
       <c r="I21">
-        <v>5.0752487182617188</v>
+        <v>5.039690017700195</v>
       </c>
       <c r="J21">
-        <v>8.4059610366821289</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.983125686645508</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
-        <v>0.54604572057723999</v>
+        <v>0.528770923614502</v>
       </c>
       <c r="B22">
-        <v>0.92727953195571899</v>
+        <v>1.041255235671997</v>
       </c>
       <c r="C22">
-        <v>1.513404369354248</v>
+        <v>1.654380917549133</v>
       </c>
       <c r="D22">
-        <v>2.067461252212524</v>
+        <v>2.320007801055908</v>
       </c>
       <c r="E22">
-        <v>2.7572250366210942</v>
+        <v>3.053170204162598</v>
       </c>
       <c r="F22">
-        <v>3.5660524368286128</v>
+        <v>3.921988725662231</v>
       </c>
       <c r="G22">
-        <v>4.4843125343322754</v>
+        <v>4.742568969726562</v>
       </c>
       <c r="H22">
-        <v>5.6210145950317383</v>
+        <v>5.915135383605957</v>
       </c>
       <c r="I22">
-        <v>7.433051586151123</v>
+        <v>7.60019063949585</v>
       </c>
       <c r="J22">
-        <v>11.713663101196291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.75913238525391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
-        <v>0.61363005638122559</v>
+        <v>0.6493108868598938</v>
       </c>
       <c r="B23">
-        <v>1.02740478515625</v>
+        <v>1.282623887062073</v>
       </c>
       <c r="C23">
-        <v>1.6543397903442381</v>
+        <v>1.979295969009399</v>
       </c>
       <c r="D23">
-        <v>2.1459400653839111</v>
+        <v>2.683341979980469</v>
       </c>
       <c r="E23">
-        <v>2.8029308319091801</v>
+        <v>3.375704526901245</v>
       </c>
       <c r="F23">
-        <v>3.5792639255523682</v>
+        <v>4.156306266784668</v>
       </c>
       <c r="G23">
-        <v>4.4913783073425293</v>
+        <v>4.902734756469727</v>
       </c>
       <c r="H23">
-        <v>5.5798521041870117</v>
+        <v>5.919058799743652</v>
       </c>
       <c r="I23">
-        <v>7.2906608581542969</v>
+        <v>7.313323974609375</v>
       </c>
       <c r="J23">
-        <v>11.241921424865721</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.06136035919189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
-        <v>0.53900676965713501</v>
+        <v>0.535047709941864</v>
       </c>
       <c r="B24">
-        <v>0.91886442899703979</v>
+        <v>0.9440071582794189</v>
       </c>
       <c r="C24">
-        <v>1.4567253589630129</v>
+        <v>1.514631509780884</v>
       </c>
       <c r="D24">
-        <v>1.969113349914551</v>
+        <v>2.048305034637451</v>
       </c>
       <c r="E24">
-        <v>2.616543292999268</v>
+        <v>2.743263244628906</v>
       </c>
       <c r="F24">
-        <v>3.474840402603149</v>
+        <v>3.581661462783813</v>
       </c>
       <c r="G24">
-        <v>4.4611058235168457</v>
+        <v>4.62563419342041</v>
       </c>
       <c r="H24">
-        <v>5.729306697845459</v>
+        <v>5.828090190887451</v>
       </c>
       <c r="I24">
-        <v>7.7276630401611328</v>
+        <v>7.716991424560547</v>
       </c>
       <c r="J24">
-        <v>13.635708808898929</v>
+        <v>13.02525329589844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>